<commit_message>
add presentation file and finish project
</commit_message>
<xml_diff>
--- a/daily report.xlsx
+++ b/daily report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>프로젝트명</t>
   </si>
@@ -215,6 +215,21 @@
   </si>
   <si>
     <t>딥러닝 이론 공부</t>
+  </si>
+  <si>
+    <t>발표 녹화, 영상촬영</t>
+  </si>
+  <si>
+    <t>ppt제작</t>
+  </si>
+  <si>
+    <t>영상편집</t>
+  </si>
+  <si>
+    <t>영상촬영</t>
+  </si>
+  <si>
+    <t>자연어 정규표현식 공부</t>
   </si>
 </sst>
 </file>
@@ -491,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -590,6 +605,9 @@
     </xf>
     <xf borderId="15" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1244,43 +1262,53 @@
       <c r="A19" s="32">
         <v>44097.0</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="34"/>
+      <c r="B19" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="34"/>
+      <c r="F19" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="34"/>
+      <c r="H19" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="34"/>
+      <c r="J19" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="K19" s="35"/>
     </row>
     <row r="20" ht="17.25" customHeight="1">
-      <c r="A20" s="35"/>
+      <c r="A20" s="36"/>
     </row>
     <row r="21" ht="17.25" customHeight="1">
-      <c r="A21" s="35"/>
+      <c r="A21" s="36"/>
     </row>
     <row r="22" ht="17.25" customHeight="1">
-      <c r="A22" s="35"/>
+      <c r="A22" s="36"/>
     </row>
     <row r="23" ht="17.25" customHeight="1">
-      <c r="A23" s="35"/>
+      <c r="A23" s="36"/>
     </row>
     <row r="24" ht="17.25" customHeight="1">
-      <c r="A24" s="35"/>
+      <c r="A24" s="36"/>
     </row>
     <row r="25" ht="17.25" customHeight="1">
-      <c r="A25" s="35"/>
+      <c r="A25" s="36"/>
     </row>
     <row r="26" ht="17.25" customHeight="1">
-      <c r="A26" s="35"/>
+      <c r="A26" s="36"/>
     </row>
     <row r="27" ht="17.25" customHeight="1">
-      <c r="A27" s="35"/>
+      <c r="A27" s="36"/>
     </row>
     <row r="28" ht="17.25" customHeight="1">
-      <c r="A28" s="35"/>
+      <c r="A28" s="36"/>
     </row>
     <row r="29" ht="17.25" customHeight="1"/>
     <row r="30" ht="17.25" customHeight="1"/>

</xml_diff>